<commit_message>
Cleaning data and WHO5 statistics
Cleaned the data, in stroop, emo, and WH=5, made descriptives, ANOVAS, and other statistical calculations.
Exported, made tables, excel sheets, and a new folder with the clean data.
</commit_message>
<xml_diff>
--- a/final_clean_data/demographics_summary.xlsx
+++ b/final_clean_data/demographics_summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Dataset</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>M</t>
-  </si>
-  <si>
-    <t>Missing sex</t>
   </si>
   <si>
     <t>Age (mean ± SD)</t>
@@ -413,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,13 +435,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2">
         <v>87</v>
@@ -455,19 +449,16 @@
       <c r="D2">
         <v>29</v>
       </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>87</v>
@@ -478,19 +469,16 @@
       <c r="D3">
         <v>29</v>
       </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>323</v>
@@ -501,14 +489,11 @@
       <c r="D4">
         <v>97</v>
       </c>
-      <c r="E4">
-        <v>0</v>
+      <c r="E4" t="s">
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>